<commit_message>
Remove historical curator notes
</commit_message>
<xml_diff>
--- a/MoD/inputs/MoD.xlsx
+++ b/MoD/inputs/MoD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/MoD/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E91492-C242-CF45-921B-45AEDA2FA88B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F961E4-4C9B-6740-B97C-D6FAD432D619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="480" windowWidth="17220" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15840" yWindow="-19560" windowWidth="17220" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MoD ontology classes" sheetId="4" r:id="rId1"/>
@@ -400,7 +400,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="295">
   <si>
     <t>ID</t>
   </si>
@@ -639,15 +639,6 @@
     <t>Electronic mode of delivery that involves the intervention recipient being given access to an e-book.</t>
   </si>
   <si>
-    <t>Definition of email to be drawn from authoritative source.</t>
-  </si>
-  <si>
-    <t>Definition of computer game to be drawn from authoritative source.</t>
-  </si>
-  <si>
-    <t>Definition of website to be drawn from authoritative source.</t>
-  </si>
-  <si>
     <t>E-book mode of delivery</t>
   </si>
   <si>
@@ -1062,12 +1053,6 @@
     <t>Can include paper, acetate, text, diagrams and photographic images.</t>
   </si>
   <si>
-    <t>Definitionof  mobile application to be drawn from authoritative source. The distinction between websites and mobile applications has become blurred with the advent of webapps.</t>
-  </si>
-  <si>
-    <t>Definition of e-book to be drawn from authoritative source.</t>
-  </si>
-  <si>
     <t>A mode of delivery that involves application of a physical stimulus to the body.</t>
   </si>
   <si>
@@ -1297,6 +1282,9 @@
   </si>
   <si>
     <t>Individual-based mode of delivery; Pair-based mode of delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The distinction between websites and mobile applications has become blurred with the advent of webapps.</t>
   </si>
 </sst>
 </file>
@@ -1733,9 +1721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1767,10 +1755,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -1825,13 +1813,13 @@
     </row>
     <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E3" s="5">
         <v>1.1000000000000001</v>
@@ -1846,12 +1834,12 @@
         <v>13</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -1860,7 +1848,7 @@
         <v>27</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>18</v>
@@ -1874,7 +1862,7 @@
     </row>
     <row r="5" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -1883,7 +1871,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>19</v>
@@ -1897,7 +1885,7 @@
     </row>
     <row r="6" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>22</v>
@@ -1906,7 +1894,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>19</v>
@@ -1920,7 +1908,7 @@
     </row>
     <row r="7" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
@@ -1929,7 +1917,7 @@
         <v>25</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>18</v>
@@ -1941,12 +1929,12 @@
         <v>13</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
@@ -1955,7 +1943,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
@@ -1969,7 +1957,7 @@
     </row>
     <row r="9" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>29</v>
@@ -1978,7 +1966,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>24</v>
@@ -1992,7 +1980,7 @@
     </row>
     <row r="10" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
@@ -2001,7 +1989,7 @@
         <v>32</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>24</v>
@@ -2018,7 +2006,7 @@
     </row>
     <row r="11" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>34</v>
@@ -2027,7 +2015,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>24</v>
@@ -2041,7 +2029,7 @@
     </row>
     <row r="12" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
@@ -2050,7 +2038,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>18</v>
@@ -2062,12 +2050,12 @@
         <v>13</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>36</v>
@@ -2076,7 +2064,7 @@
         <v>56</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>37</v>
@@ -2093,7 +2081,7 @@
     </row>
     <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
@@ -2102,7 +2090,7 @@
         <v>41</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>37</v>
@@ -2116,7 +2104,7 @@
     </row>
     <row r="15" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>40</v>
@@ -2125,7 +2113,7 @@
         <v>42</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>37</v>
@@ -2139,7 +2127,7 @@
     </row>
     <row r="16" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>43</v>
@@ -2148,7 +2136,7 @@
         <v>44</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>37</v>
@@ -2162,7 +2150,7 @@
     </row>
     <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>67</v>
@@ -2171,7 +2159,7 @@
         <v>46</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>37</v>
@@ -2188,7 +2176,7 @@
     </row>
     <row r="18" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>47</v>
@@ -2197,7 +2185,7 @@
         <v>48</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>37</v>
@@ -2214,7 +2202,7 @@
     </row>
     <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>50</v>
@@ -2223,7 +2211,7 @@
         <v>51</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>37</v>
@@ -2235,21 +2223,21 @@
         <v>13</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>37</v>
@@ -2263,7 +2251,7 @@
     </row>
     <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>53</v>
@@ -2272,7 +2260,7 @@
         <v>52</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>37</v>
@@ -2289,7 +2277,7 @@
     </row>
     <row r="22" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>55</v>
@@ -2298,7 +2286,7 @@
         <v>58</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>37</v>
@@ -2315,16 +2303,16 @@
     </row>
     <row r="23" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>37</v>
@@ -2336,21 +2324,21 @@
         <v>13</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>70</v>
@@ -2367,16 +2355,16 @@
     </row>
     <row r="25" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>70</v>
@@ -2390,16 +2378,16 @@
     </row>
     <row r="26" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>70</v>
@@ -2411,12 +2399,12 @@
         <v>13</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>72</v>
@@ -2425,7 +2413,7 @@
         <v>73</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>37</v>
@@ -2436,13 +2424,10 @@
       <c r="H27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="28" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>74</v>
@@ -2451,7 +2436,7 @@
         <v>75</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>37</v>
@@ -2462,22 +2447,19 @@
       <c r="H28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="29" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>37</v>
@@ -2488,22 +2470,19 @@
       <c r="H29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>37</v>
@@ -2515,21 +2494,21 @@
         <v>13</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>220</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>37</v>
@@ -2540,13 +2519,10 @@
       <c r="H31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>221</v>
-      </c>
     </row>
     <row r="32" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>60</v>
@@ -2555,7 +2531,7 @@
         <v>61</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>18</v>
@@ -2569,7 +2545,7 @@
     </row>
     <row r="33" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>63</v>
@@ -2578,7 +2554,7 @@
         <v>62</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>18</v>
@@ -2592,7 +2568,7 @@
     </row>
     <row r="34" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>64</v>
@@ -2601,7 +2577,7 @@
         <v>65</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>18</v>
@@ -2615,19 +2591,19 @@
     </row>
     <row r="35" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E35" s="5">
         <v>1.2</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>6</v>
@@ -2636,27 +2612,27 @@
         <v>13</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E36" s="5">
         <v>1.3</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>6</v>
@@ -2665,24 +2641,24 @@
         <v>13</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>6</v>
@@ -2693,19 +2669,19 @@
     </row>
     <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>6</v>
@@ -2716,19 +2692,19 @@
     </row>
     <row r="39" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>6</v>
@@ -2739,19 +2715,19 @@
     </row>
     <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>6</v>
@@ -2762,19 +2738,19 @@
     </row>
     <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>6</v>
@@ -2785,19 +2761,19 @@
     </row>
     <row r="42" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>6</v>
@@ -2808,19 +2784,19 @@
     </row>
     <row r="43" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>6</v>
@@ -2831,19 +2807,19 @@
     </row>
     <row r="44" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>6</v>
@@ -2854,19 +2830,19 @@
     </row>
     <row r="45" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>6</v>
@@ -2877,19 +2853,19 @@
     </row>
     <row r="46" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>6</v>
@@ -2900,19 +2876,19 @@
     </row>
     <row r="47" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>6</v>
@@ -2923,19 +2899,19 @@
     </row>
     <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>6</v>
@@ -2944,24 +2920,24 @@
         <v>13</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>6</v>
@@ -2970,24 +2946,24 @@
         <v>13</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>6</v>
@@ -2998,19 +2974,19 @@
     </row>
     <row r="51" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>6</v>
@@ -3019,24 +2995,24 @@
         <v>13</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>6</v>
@@ -3047,19 +3023,19 @@
     </row>
     <row r="53" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>6</v>
@@ -3070,19 +3046,19 @@
     </row>
     <row r="54" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>6</v>
@@ -3091,24 +3067,24 @@
         <v>13</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>6</v>
@@ -3119,19 +3095,19 @@
     </row>
     <row r="56" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E56" s="5">
         <v>1.4</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>6</v>
@@ -3140,27 +3116,27 @@
         <v>13</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:12" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E57" s="7">
         <v>1.5</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>6</v>
@@ -3171,22 +3147,22 @@
     </row>
     <row r="58" spans="1:12" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E58" s="7">
         <v>1.6</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>6</v>
@@ -3197,22 +3173,22 @@
     </row>
     <row r="59" spans="1:12" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B59" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="D59" s="6" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E59" s="7">
         <v>1.7</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>6</v>
@@ -3223,22 +3199,22 @@
     </row>
     <row r="60" spans="1:12" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E60" s="9">
         <v>1.8</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>6</v>
@@ -3249,22 +3225,22 @@
     </row>
     <row r="61" spans="1:12" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E61" s="9">
         <v>1.9</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>6</v>
@@ -3275,22 +3251,22 @@
     </row>
     <row r="62" spans="1:12" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G62" s="10" t="s">
         <v>6</v>
@@ -3301,22 +3277,22 @@
     </row>
     <row r="63" spans="1:12" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E63" s="11">
         <v>1.1100000000000001</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G63" s="10" t="s">
         <v>6</v>
@@ -3327,22 +3303,22 @@
     </row>
     <row r="64" spans="1:12" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E64" s="13">
         <v>1.1200000000000001</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G64" s="12" t="s">
         <v>6</v>
@@ -3353,22 +3329,22 @@
     </row>
     <row r="65" spans="1:12" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E65" s="13">
         <v>1.1299999999999999</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G65" s="12" t="s">
         <v>6</v>
@@ -3379,19 +3355,19 @@
     </row>
     <row r="66" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E66" s="5">
         <v>1.1399999999999999</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>6</v>
@@ -3400,27 +3376,27 @@
         <v>13</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E67" s="5">
         <v>1.1499999999999999</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>6</v>
@@ -3429,7 +3405,7 @@
         <v>13</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add columns for online editing support
</commit_message>
<xml_diff>
--- a/MoD/inputs/MoD.xlsx
+++ b/MoD/inputs/MoD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/MoD/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F961E4-4C9B-6740-B97C-D6FAD432D619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820638FF-DF95-2A4F-9420-22FB727C7C79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15840" yWindow="-19560" windowWidth="17220" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="2700" windowWidth="22060" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MoD ontology classes" sheetId="4" r:id="rId1"/>
@@ -400,7 +400,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="300">
   <si>
     <t>ID</t>
   </si>
@@ -1285,6 +1285,21 @@
   </si>
   <si>
     <t xml:space="preserve"> The distinction between websites and mobile applications has become blurred with the advent of webapps.</t>
+  </si>
+  <si>
+    <t>Curator</t>
+  </si>
+  <si>
+    <t>Curation status</t>
+  </si>
+  <si>
+    <t>To be reviewed by</t>
+  </si>
+  <si>
+    <t>Reviewer query</t>
+  </si>
+  <si>
+    <t>Discussed</t>
   </si>
 </sst>
 </file>
@@ -1719,11 +1734,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M67"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O68" sqref="O68:O75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1741,10 +1756,14 @@
     <col min="11" max="11" width="23.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="44.83203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="44.1640625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="1"/>
+    <col min="14" max="14" width="17.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1784,8 +1803,20 @@
       <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="N1" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1810,8 +1841,11 @@
       <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="O2" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>225</v>
       </c>
@@ -1836,8 +1870,11 @@
       <c r="L3" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O3" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>226</v>
       </c>
@@ -1859,8 +1896,11 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O4" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>227</v>
       </c>
@@ -1882,8 +1922,11 @@
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="O5" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>228</v>
       </c>
@@ -1905,8 +1948,11 @@
       <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O6" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>229</v>
       </c>
@@ -1931,8 +1977,11 @@
       <c r="L7" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O7" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>230</v>
       </c>
@@ -1954,8 +2003,11 @@
       <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O8" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>231</v>
       </c>
@@ -1977,8 +2029,11 @@
       <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O9" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -2003,8 +2058,11 @@
       <c r="L10" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="O10" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>233</v>
       </c>
@@ -2026,8 +2084,11 @@
       <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="O11" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>234</v>
       </c>
@@ -2052,8 +2113,11 @@
       <c r="J12" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O12" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>235</v>
       </c>
@@ -2078,8 +2142,11 @@
       <c r="L13" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O13" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>236</v>
       </c>
@@ -2101,8 +2168,11 @@
       <c r="H14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O14" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>237</v>
       </c>
@@ -2124,8 +2194,11 @@
       <c r="H15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="O15" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>238</v>
       </c>
@@ -2147,8 +2220,11 @@
       <c r="H16" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O16" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>239</v>
       </c>
@@ -2173,8 +2249,11 @@
       <c r="L17" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O17" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>240</v>
       </c>
@@ -2199,8 +2278,11 @@
       <c r="L18" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O18" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>241</v>
       </c>
@@ -2225,8 +2307,11 @@
       <c r="L19" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O19" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>242</v>
       </c>
@@ -2248,8 +2333,11 @@
       <c r="H20" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O20" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>243</v>
       </c>
@@ -2274,8 +2362,11 @@
       <c r="L21" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O21" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>244</v>
       </c>
@@ -2300,8 +2391,11 @@
       <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O22" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>245</v>
       </c>
@@ -2326,8 +2420,11 @@
       <c r="J23" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O23" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>246</v>
       </c>
@@ -2352,8 +2449,11 @@
       <c r="L24" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O24" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>247</v>
       </c>
@@ -2375,8 +2475,11 @@
       <c r="H25" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O25" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>248</v>
       </c>
@@ -2401,8 +2504,11 @@
       <c r="L26" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O26" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>249</v>
       </c>
@@ -2424,8 +2530,11 @@
       <c r="H27" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O27" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>250</v>
       </c>
@@ -2447,8 +2556,11 @@
       <c r="H28" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O28" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>251</v>
       </c>
@@ -2470,8 +2582,11 @@
       <c r="H29" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O29" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>252</v>
       </c>
@@ -2496,8 +2611,11 @@
       <c r="J30" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O30" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>253</v>
       </c>
@@ -2519,8 +2637,11 @@
       <c r="H31" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O31" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>254</v>
       </c>
@@ -2542,8 +2663,11 @@
       <c r="H32" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O32" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>255</v>
       </c>
@@ -2565,8 +2689,11 @@
       <c r="H33" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O33" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>256</v>
       </c>
@@ -2588,8 +2715,11 @@
       <c r="H34" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O34" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>257</v>
       </c>
@@ -2617,8 +2747,11 @@
       <c r="L35" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O35" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>258</v>
       </c>
@@ -2643,8 +2776,11 @@
       <c r="J36" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O36" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>259</v>
       </c>
@@ -2666,8 +2802,11 @@
       <c r="H37" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O37" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>260</v>
       </c>
@@ -2689,8 +2828,11 @@
       <c r="H38" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O38" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>261</v>
       </c>
@@ -2712,8 +2854,11 @@
       <c r="H39" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O39" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>262</v>
       </c>
@@ -2735,8 +2880,11 @@
       <c r="H40" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O40" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>263</v>
       </c>
@@ -2758,8 +2906,11 @@
       <c r="H41" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O41" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>264</v>
       </c>
@@ -2781,8 +2932,11 @@
       <c r="H42" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O42" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>265</v>
       </c>
@@ -2804,8 +2958,11 @@
       <c r="H43" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O43" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>266</v>
       </c>
@@ -2827,8 +2984,11 @@
       <c r="H44" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O44" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>267</v>
       </c>
@@ -2850,8 +3010,11 @@
       <c r="H45" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O45" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>268</v>
       </c>
@@ -2873,8 +3036,11 @@
       <c r="H46" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O46" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>269</v>
       </c>
@@ -2896,8 +3062,11 @@
       <c r="H47" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O47" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>270</v>
       </c>
@@ -2922,8 +3091,11 @@
       <c r="L48" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O48" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>271</v>
       </c>
@@ -2948,8 +3120,11 @@
       <c r="L49" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O49" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>272</v>
       </c>
@@ -2971,8 +3146,11 @@
       <c r="H50" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O50" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>273</v>
       </c>
@@ -2997,8 +3175,11 @@
       <c r="K51" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O51" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>274</v>
       </c>
@@ -3020,8 +3201,11 @@
       <c r="H52" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O52" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>275</v>
       </c>
@@ -3043,8 +3227,11 @@
       <c r="H53" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O53" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>276</v>
       </c>
@@ -3069,8 +3256,11 @@
       <c r="L54" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O54" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>277</v>
       </c>
@@ -3092,8 +3282,11 @@
       <c r="H55" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O55" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>278</v>
       </c>
@@ -3118,8 +3311,11 @@
       <c r="L56" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O56" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>279</v>
       </c>
@@ -3144,8 +3340,11 @@
       <c r="H57" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O57" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>280</v>
       </c>
@@ -3170,8 +3369,11 @@
       <c r="H58" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O58" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>281</v>
       </c>
@@ -3196,8 +3398,11 @@
       <c r="H59" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O59" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>282</v>
       </c>
@@ -3222,8 +3427,11 @@
       <c r="H60" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O60" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>283</v>
       </c>
@@ -3248,8 +3456,11 @@
       <c r="H61" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O61" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>284</v>
       </c>
@@ -3274,8 +3485,11 @@
       <c r="H62" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O62" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>285</v>
       </c>
@@ -3300,8 +3514,11 @@
       <c r="H63" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O63" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>286</v>
       </c>
@@ -3326,8 +3543,11 @@
       <c r="H64" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="O64" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>287</v>
       </c>
@@ -3352,8 +3572,11 @@
       <c r="H65" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O65" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>288</v>
       </c>
@@ -3381,8 +3604,11 @@
       <c r="L66" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O66" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>289</v>
       </c>
@@ -3406,6 +3632,9 @@
       </c>
       <c r="L67" s="1" t="s">
         <v>151</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>